<commit_message>
Using key in displayId construction before processing
</commit_message>
<xml_diff>
--- a/src/test/resources/ed/biordm/sbol/toolkit/transform/annot_test.xlsx
+++ b/src/test/resources/ed/biordm/sbol/toolkit/transform/annot_test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>display_id</t>
   </si>
@@ -42,9 +42,6 @@
     <t>target gene {name}</t>
   </si>
   <si>
-    <t>cs0002_slr0612</t>
-  </si>
-  <si>
     <t>cs0003_slr0613</t>
   </si>
   <si>
@@ -58,6 +55,12 @@
   </si>
   <si>
     <t>{key}</t>
+  </si>
+  <si>
+    <t>slr0612</t>
+  </si>
+  <si>
+    <t>cs0002_{key}</t>
   </si>
 </sst>
 </file>
@@ -378,7 +381,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,13 +397,13 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -411,7 +414,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -420,7 +423,7 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -428,24 +431,27 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
       </c>
       <c r="C4">
         <v>3</v>

</xml_diff>